<commit_message>
Add free time file
</commit_message>
<xml_diff>
--- a/Thoi-gian-roi.xlsx
+++ b/Thoi-gian-roi.xlsx
@@ -54,12 +54,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,14 +92,136 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,135 +234,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -263,181 +256,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,16 +475,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,16 +505,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,21 +533,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,159 +548,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1041,7 +1034,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="4"/>
@@ -1071,7 +1064,9 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1080,7 +1075,9 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1089,7 +1086,9 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1098,7 +1097,9 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1107,7 +1108,9 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1116,7 +1119,9 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1125,7 +1130,9 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>

</xml_diff>